<commit_message>
update fix akun upload excel
</commit_message>
<xml_diff>
--- a/public/template/template_upload_karyawan.xlsx
+++ b/public/template/template_upload_karyawan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36D4EA-F537-4EC0-8632-1BA8D3577341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD69D427-2DA6-4541-B555-95437FD95ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>No KTP</t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>Nomor Induk Karyawan (Mandatory)</t>
+  </si>
+  <si>
+    <t>Username Akun System (Mandatory)</t>
+  </si>
+  <si>
+    <t>Email Akun System (Mandatory)</t>
+  </si>
+  <si>
+    <t>Password Akun System (Mandatory)</t>
+  </si>
+  <si>
+    <t>Ex : fathan@tcf.com</t>
+  </si>
+  <si>
+    <t>Ex : FA1722</t>
+  </si>
+  <si>
+    <t>Ex : passwordakun123</t>
   </si>
 </sst>
 </file>
@@ -168,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,14 +209,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D0E4EC-B375-444C-A099-75B908B6C530}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,9 +568,12 @@
     <col min="15" max="15" width="19.5703125" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
     <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.7109375" customWidth="1"/>
+    <col min="19" max="19" width="37.140625" customWidth="1"/>
+    <col min="20" max="20" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -592,8 +625,17 @@
       <c r="Q1" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -644,6 +686,15 @@
       </c>
       <c r="Q2" t="s">
         <v>26</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finishing upload karyawan with posisi
</commit_message>
<xml_diff>
--- a/public/template/template_upload_karyawan.xlsx
+++ b/public/template/template_upload_karyawan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD69D427-2DA6-4541-B555-95437FD95ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5B8E90-2FBF-4901-B432-A64F3C9E4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>No KTP</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Ex : Karawang</t>
   </si>
   <si>
-    <t>Ex : 2002-02-17</t>
-  </si>
-  <si>
     <t>Ex : sikasep@gmail.com</t>
   </si>
   <si>
@@ -151,6 +148,21 @@
   </si>
   <si>
     <t>Ex : passwordakun123</t>
+  </si>
+  <si>
+    <t>Nama Posisi</t>
+  </si>
+  <si>
+    <t>Ex : 17/02/2002</t>
+  </si>
+  <si>
+    <t>Ex : 01/01/2024</t>
+  </si>
+  <si>
+    <t>(Wajib sama dengan data dari database, boleh lebih dari 1 dengan separator koma " , " )</t>
+  </si>
+  <si>
+    <t>Tanggal Mulai Bekerja</t>
   </si>
 </sst>
 </file>
@@ -166,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +194,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -224,11 +242,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D0E4EC-B375-444C-A099-75B908B6C530}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,14 +591,16 @@
     <col min="18" max="18" width="33.7109375" customWidth="1"/>
     <col min="19" max="19" width="37.140625" customWidth="1"/>
     <col min="20" max="20" width="36" customWidth="1"/>
+    <col min="21" max="21" width="31.42578125" customWidth="1"/>
+    <col min="22" max="22" width="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -605,7 +627,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>8</v>
@@ -623,78 +645,90 @@
         <v>12</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>35</v>
+      <c r="U1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
       <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
       <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
         <v>36</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>37</v>
       </c>
-      <c r="T2" t="s">
-        <v>38</v>
+      <c r="U2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finishing add more field in Karyawan
</commit_message>
<xml_diff>
--- a/public/template/template_upload_karyawan.xlsx
+++ b/public/template/template_upload_karyawan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5B8E90-2FBF-4901-B432-A64F3C9E4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ECB78B-32E5-4372-A9AC-B0F254067A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
   </bookViews>
@@ -34,46 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
-  <si>
-    <t>No KTP</t>
-  </si>
-  <si>
-    <t>NIK</t>
-  </si>
-  <si>
-    <t>Tempat Lahir</t>
-  </si>
-  <si>
-    <t>Tanggal Lahir</t>
-  </si>
-  <si>
-    <t>Alamat</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>No.HP</t>
-  </si>
-  <si>
-    <t>Gol. Darah</t>
-  </si>
-  <si>
-    <t>Agama</t>
-  </si>
-  <si>
-    <t>Status Keluarga</t>
-  </si>
-  <si>
-    <t>NPWP</t>
-  </si>
-  <si>
-    <t>No. BPJS KS</t>
-  </si>
-  <si>
-    <t>No. BPJS KT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>Ex : Karawang</t>
   </si>
@@ -81,21 +42,12 @@
     <t>Ex : sikasep@gmail.com</t>
   </si>
   <si>
-    <t>Ex : 321501180280004</t>
-  </si>
-  <si>
     <t>Ex : 321501180280345</t>
   </si>
   <si>
-    <t>Ex : Jl.NaikGaji No.2025</t>
-  </si>
-  <si>
     <t>Ex : ISLAM / KATOLIK / KRISTEN / KONGHUCU / HINDU / BUDHA / PROTESTAN / LAINNYA</t>
   </si>
   <si>
-    <t>Ex : MENIKAH / LAJANG</t>
-  </si>
-  <si>
     <t>Ex : L / P</t>
   </si>
   <si>
@@ -111,48 +63,18 @@
     <t>(isi sesuai no BPJS)</t>
   </si>
   <si>
-    <t>Ex : 12 (Range dari 0 - 12)</t>
-  </si>
-  <si>
-    <t>Nama (Mandatory)</t>
-  </si>
-  <si>
-    <t>Jenis Kelamin  (Mandatory)</t>
-  </si>
-  <si>
-    <t>Sisa Cuti (Mandatory)</t>
-  </si>
-  <si>
     <t>Ex : 628987336533</t>
   </si>
   <si>
     <t>Ex : 480.030524</t>
   </si>
   <si>
-    <t>Nomor Induk Karyawan (Mandatory)</t>
-  </si>
-  <si>
-    <t>Username Akun System (Mandatory)</t>
-  </si>
-  <si>
-    <t>Email Akun System (Mandatory)</t>
-  </si>
-  <si>
-    <t>Password Akun System (Mandatory)</t>
-  </si>
-  <si>
-    <t>Ex : fathan@tcf.com</t>
-  </si>
-  <si>
     <t>Ex : FA1722</t>
   </si>
   <si>
     <t>Ex : passwordakun123</t>
   </si>
   <si>
-    <t>Nama Posisi</t>
-  </si>
-  <si>
     <t>Ex : 17/02/2002</t>
   </si>
   <si>
@@ -162,14 +84,134 @@
     <t>(Wajib sama dengan data dari database, boleh lebih dari 1 dengan separator koma " , " )</t>
   </si>
   <si>
-    <t>Tanggal Mulai Bekerja</t>
+    <t>Domisili *</t>
+  </si>
+  <si>
+    <t>Alamat *</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin  *</t>
+  </si>
+  <si>
+    <t>Nama *</t>
+  </si>
+  <si>
+    <t>Nomor Induk Karyawan *</t>
+  </si>
+  <si>
+    <t>Tempat Lahir *</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir *</t>
+  </si>
+  <si>
+    <t>Status Keluarga *</t>
+  </si>
+  <si>
+    <t>Kategori Keluarga *</t>
+  </si>
+  <si>
+    <t>Agama *</t>
+  </si>
+  <si>
+    <t>No. KK *</t>
+  </si>
+  <si>
+    <t>NIK/No. KTP*</t>
+  </si>
+  <si>
+    <t>NPWP *</t>
+  </si>
+  <si>
+    <t>No. BPJS Ketenagakerjaan *</t>
+  </si>
+  <si>
+    <t>No. BPJS Kesehatan *</t>
+  </si>
+  <si>
+    <t>No. HP *</t>
+  </si>
+  <si>
+    <t>Tanggal Bergabung *</t>
+  </si>
+  <si>
+    <t>Pendidikan Terakhir *</t>
+  </si>
+  <si>
+    <t>Jurusan *</t>
+  </si>
+  <si>
+    <t>Nama Ibu Kandung *</t>
+  </si>
+  <si>
+    <t>Nama Bank *</t>
+  </si>
+  <si>
+    <t>No. Rekening *</t>
+  </si>
+  <si>
+    <t>Atas Nama Rekening *</t>
+  </si>
+  <si>
+    <t>Email Pribadi (Gmail) *</t>
+  </si>
+  <si>
+    <t>Ex : fathan@tcf.com (jika tidak ada, gunakan @tcf.com)</t>
+  </si>
+  <si>
+    <t>Email Perusahaan *</t>
+  </si>
+  <si>
+    <t>Username Akun System *</t>
+  </si>
+  <si>
+    <t>Password Akun System *</t>
+  </si>
+  <si>
+    <t>Ex : Jl.Tricentrum No.2025</t>
+  </si>
+  <si>
+    <t>Ex : MENIKAH / BELUM MENIKAH / CERAI</t>
+  </si>
+  <si>
+    <t>Ex : TK0 / TK1 / K0 / K3</t>
+  </si>
+  <si>
+    <t>Ex : 321501180280444</t>
+  </si>
+  <si>
+    <t>Ex : SD/SMP/SMA/D1/D2/D3/S1/S2/S3</t>
+  </si>
+  <si>
+    <t>Ex : Manajemen</t>
+  </si>
+  <si>
+    <t>(Isi dengan huruf Kapital)</t>
+  </si>
+  <si>
+    <t>Ex : MANDIRI / BRI / BCA / BSI / BNI</t>
+  </si>
+  <si>
+    <t>Ex : 170654123</t>
+  </si>
+  <si>
+    <t>Nama Posisi *</t>
+  </si>
+  <si>
+    <t>Golongan Darah *</t>
+  </si>
+  <si>
+    <t>No. Telp Darurat *</t>
+  </si>
+  <si>
+    <t>Ex : 62845663255</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +219,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,24 +249,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -227,30 +282,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,172 +609,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D0E4EC-B375-444C-A099-75B908B6C530}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="49.85546875" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" customWidth="1"/>
-    <col min="12" max="12" width="76.85546875" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="33.7109375" customWidth="1"/>
-    <col min="19" max="19" width="37.140625" customWidth="1"/>
-    <col min="20" max="20" width="36" customWidth="1"/>
-    <col min="21" max="21" width="31.42578125" customWidth="1"/>
-    <col min="22" max="22" width="86" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="49.85546875" customWidth="1"/>
+    <col min="9" max="9" width="38.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="11" max="11" width="80" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" customWidth="1"/>
+    <col min="13" max="13" width="76.85546875" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1"/>
+    <col min="15" max="15" width="29" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.140625" customWidth="1"/>
+    <col min="21" max="21" width="36" customWidth="1"/>
+    <col min="22" max="22" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.42578125" customWidth="1"/>
+    <col min="24" max="24" width="25" customWidth="1"/>
+    <col min="25" max="26" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:30" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="Z2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="AA2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="AC2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
+      <c r="AD2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major update di upload karyawan, tampilan menu, dan minor2 update lainnya
</commit_message>
<xml_diff>
--- a/public/template/template_upload_karyawan.xlsx
+++ b/public/template/template_upload_karyawan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ECB78B-32E5-4372-A9AC-B0F254067A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C73136-97AB-49CD-962A-BFDDF092E8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Ex : Karawang</t>
   </si>
@@ -205,6 +205,27 @@
   </si>
   <si>
     <t>Ex : 62845663255</t>
+  </si>
+  <si>
+    <t>Jatah Cuti Pribadi *</t>
+  </si>
+  <si>
+    <t>Jatah Cuti Bersama *</t>
+  </si>
+  <si>
+    <t>Jatah Cuti Tahun Lalu *</t>
+  </si>
+  <si>
+    <t>Isi dengan angka saja</t>
+  </si>
+  <si>
+    <t>Ex : 01/02/2025</t>
+  </si>
+  <si>
+    <t>Expired Date Cuti Tahun Lalu *</t>
+  </si>
+  <si>
+    <t>Hutang Cuti *</t>
   </si>
 </sst>
 </file>
@@ -287,13 +308,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -609,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D0E4EC-B375-444C-A099-75B908B6C530}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,9 +665,14 @@
     <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -738,8 +763,23 @@
       <c r="AD1" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="AE1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -815,7 +855,7 @@
       <c r="Y2" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" t="s">
         <v>5</v>
       </c>
       <c r="AA2" t="s">
@@ -829,6 +869,21 @@
       </c>
       <c r="AD2" t="s">
         <v>56</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mayor update pengurangan cuti khusus
</commit_message>
<xml_diff>
--- a/public/template/template_upload_karyawan.xlsx
+++ b/public/template/template_upload_karyawan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C73136-97AB-49CD-962A-BFDDF092E8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A75E787-F1DF-4509-88F8-9A294533731E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Ex : 01/01/2024</t>
   </si>
   <si>
-    <t>(Wajib sama dengan data dari database, boleh lebih dari 1 dengan separator koma " , " )</t>
-  </si>
-  <si>
     <t>Domisili *</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>Hutang Cuti *</t>
+  </si>
+  <si>
+    <t>(Wajib sama dengan data dari database, hanya boleh mengisi 1 Posisi utama sebagai inisialisasi )</t>
   </si>
 </sst>
 </file>
@@ -631,14 +631,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D0E4EC-B375-444C-A099-75B908B6C530}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI4" sqref="AI4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.42578125" customWidth="1"/>
+    <col min="2" max="2" width="96.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.140625" customWidth="1"/>
     <col min="4" max="4" width="29.85546875" customWidth="1"/>
     <col min="5" max="6" width="33" customWidth="1"/>
@@ -674,109 +674,109 @@
   <sheetData>
     <row r="1" spans="1:35" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="AE1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AG1" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="AH1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -793,10 +793,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -805,16 +805,16 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
         <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
@@ -835,22 +835,22 @@
         <v>14</v>
       </c>
       <c r="S2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" t="s">
         <v>48</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>49</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>50</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" t="s">
         <v>51</v>
-      </c>
-      <c r="W2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" t="s">
-        <v>52</v>
       </c>
       <c r="Y2" t="s">
         <v>1</v>
@@ -859,7 +859,7 @@
         <v>5</v>
       </c>
       <c r="AA2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB2" t="s">
         <v>11</v>
@@ -868,22 +868,22 @@
         <v>12</v>
       </c>
       <c r="AD2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AE2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" t="s">
         <v>60</v>
       </c>
-      <c r="AF2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>61</v>
-      </c>
       <c r="AI2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update upload karyawan menggunakan job
</commit_message>
<xml_diff>
--- a/public/template/template_upload_karyawan.xlsx
+++ b/public/template/template_upload_karyawan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ict-d\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A75E787-F1DF-4509-88F8-9A294533731E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10A50CC-078F-448B-B9F6-A2B578EEBEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Ex : Karawang</t>
   </si>
@@ -81,99 +81,12 @@
     <t>Ex : 01/01/2024</t>
   </si>
   <si>
-    <t>Domisili *</t>
-  </si>
-  <si>
-    <t>Alamat *</t>
-  </si>
-  <si>
-    <t>Jenis Kelamin  *</t>
-  </si>
-  <si>
-    <t>Nama *</t>
-  </si>
-  <si>
-    <t>Nomor Induk Karyawan *</t>
-  </si>
-  <si>
-    <t>Tempat Lahir *</t>
-  </si>
-  <si>
-    <t>Tanggal Lahir *</t>
-  </si>
-  <si>
-    <t>Status Keluarga *</t>
-  </si>
-  <si>
-    <t>Kategori Keluarga *</t>
-  </si>
-  <si>
-    <t>Agama *</t>
-  </si>
-  <si>
-    <t>No. KK *</t>
-  </si>
-  <si>
-    <t>NIK/No. KTP*</t>
-  </si>
-  <si>
-    <t>NPWP *</t>
-  </si>
-  <si>
-    <t>No. BPJS Ketenagakerjaan *</t>
-  </si>
-  <si>
-    <t>No. BPJS Kesehatan *</t>
-  </si>
-  <si>
-    <t>No. HP *</t>
-  </si>
-  <si>
-    <t>Tanggal Bergabung *</t>
-  </si>
-  <si>
-    <t>Pendidikan Terakhir *</t>
-  </si>
-  <si>
-    <t>Jurusan *</t>
-  </si>
-  <si>
-    <t>Nama Ibu Kandung *</t>
-  </si>
-  <si>
-    <t>Nama Bank *</t>
-  </si>
-  <si>
-    <t>No. Rekening *</t>
-  </si>
-  <si>
-    <t>Atas Nama Rekening *</t>
-  </si>
-  <si>
-    <t>Email Pribadi (Gmail) *</t>
-  </si>
-  <si>
-    <t>Ex : fathan@tcf.com (jika tidak ada, gunakan @tcf.com)</t>
-  </si>
-  <si>
-    <t>Email Perusahaan *</t>
-  </si>
-  <si>
-    <t>Username Akun System *</t>
-  </si>
-  <si>
-    <t>Password Akun System *</t>
-  </si>
-  <si>
     <t>Ex : Jl.Tricentrum No.2025</t>
   </si>
   <si>
     <t>Ex : MENIKAH / BELUM MENIKAH / CERAI</t>
   </si>
   <si>
-    <t>Ex : TK0 / TK1 / K0 / K3</t>
-  </si>
-  <si>
     <t>Ex : 321501180280444</t>
   </si>
   <si>
@@ -192,40 +105,139 @@
     <t>Ex : 170654123</t>
   </si>
   <si>
-    <t>Nama Posisi *</t>
-  </si>
-  <si>
-    <t>Golongan Darah *</t>
-  </si>
-  <si>
-    <t>No. Telp Darurat *</t>
-  </si>
-  <si>
     <t>Ex : 62845663255</t>
   </si>
   <si>
-    <t>Jatah Cuti Pribadi *</t>
-  </si>
-  <si>
-    <t>Jatah Cuti Bersama *</t>
-  </si>
-  <si>
-    <t>Jatah Cuti Tahun Lalu *</t>
-  </si>
-  <si>
     <t>Isi dengan angka saja</t>
   </si>
   <si>
     <t>Ex : 01/02/2025</t>
   </si>
   <si>
-    <t>Expired Date Cuti Tahun Lalu *</t>
-  </si>
-  <si>
-    <t>Hutang Cuti *</t>
-  </si>
-  <si>
     <t>(Wajib sama dengan data dari database, hanya boleh mengisi 1 Posisi utama sebagai inisialisasi )</t>
+  </si>
+  <si>
+    <t>(Boleh dikosongkan, hanya untuk kebutuhan VLOOKUP)</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin (Option)</t>
+  </si>
+  <si>
+    <t>Nama (Free Text)</t>
+  </si>
+  <si>
+    <t>Alamat (Free Text)</t>
+  </si>
+  <si>
+    <t>Domisili (Free Text)</t>
+  </si>
+  <si>
+    <t>Tempat Lahir (Free Text)</t>
+  </si>
+  <si>
+    <t>Status Keluarga (Option)</t>
+  </si>
+  <si>
+    <t>Ex : TK0, TK1, TK2, TK3, K0, K1, K2, K3</t>
+  </si>
+  <si>
+    <t>Kategori Keluarga (Option)</t>
+  </si>
+  <si>
+    <t>Agama (Free Text)</t>
+  </si>
+  <si>
+    <t>No. KK (Numeric)</t>
+  </si>
+  <si>
+    <t>NIK/No. KTP (Numeric)</t>
+  </si>
+  <si>
+    <t>NPWP (Free Text)</t>
+  </si>
+  <si>
+    <t>No. BPJS Ketenagakerjaan (Numeric)</t>
+  </si>
+  <si>
+    <t>No. BPJS Kesehatan (Numeric)</t>
+  </si>
+  <si>
+    <t>No. HP (Numeric &amp; Unique)</t>
+  </si>
+  <si>
+    <t>Nomor Induk Karyawan (Unique)</t>
+  </si>
+  <si>
+    <t>ID Posisi (Numeric)</t>
+  </si>
+  <si>
+    <t>Nama Posisi (Free Text)</t>
+  </si>
+  <si>
+    <t>Pendidikan Terakhir (Free Text)</t>
+  </si>
+  <si>
+    <t>Jurusan (Free Text)</t>
+  </si>
+  <si>
+    <t>Nama Ibu Kandung (Free Text)</t>
+  </si>
+  <si>
+    <t>Nama Bank (Free Text)</t>
+  </si>
+  <si>
+    <t>Atas Nama Rekening (Free Text)</t>
+  </si>
+  <si>
+    <t>No. Rekening (Numeric)</t>
+  </si>
+  <si>
+    <t>Email Pribadi (Email &amp; Unique)</t>
+  </si>
+  <si>
+    <t>Golongan Darah (Option)</t>
+  </si>
+  <si>
+    <t>Email Perusahaan (Email &amp; Unique)</t>
+  </si>
+  <si>
+    <t>Ex : jika tidak ada maka gunakan email pribadi</t>
+  </si>
+  <si>
+    <t>Username Akun System (Unique)</t>
+  </si>
+  <si>
+    <t>Password Akun System (Free Text)</t>
+  </si>
+  <si>
+    <t>No. Telp Darurat (Numeric)</t>
+  </si>
+  <si>
+    <t>Jatah Cuti Pribadi (Numeric)</t>
+  </si>
+  <si>
+    <t>Jatah Cuti Bersama (Numeric)</t>
+  </si>
+  <si>
+    <t>Jatah Cuti Tahun Lalu (Numeric)</t>
+  </si>
+  <si>
+    <t>Expired Date Cuti Tahun Lalu (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Hutang Cuti (Numeric)</t>
+  </si>
+  <si>
+    <t>Ex: 153</t>
+  </si>
+  <si>
+    <t>PIN Fingerprint (String)</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Tanggal Bergabung (dd/mm/yyyy)</t>
   </si>
 </sst>
 </file>
@@ -261,7 +273,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +288,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,12 +326,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -629,261 +648,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D0E4EC-B375-444C-A099-75B908B6C530}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="49.85546875" customWidth="1"/>
-    <col min="9" max="9" width="38.28515625" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" customWidth="1"/>
-    <col min="11" max="11" width="80" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.85546875" customWidth="1"/>
-    <col min="13" max="13" width="76.85546875" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" customWidth="1"/>
-    <col min="15" max="15" width="29" customWidth="1"/>
-    <col min="16" max="16" width="28.140625" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.140625" customWidth="1"/>
-    <col min="21" max="21" width="36" customWidth="1"/>
-    <col min="22" max="22" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.42578125" customWidth="1"/>
-    <col min="24" max="24" width="25" customWidth="1"/>
-    <col min="25" max="26" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+    <col min="5" max="5" width="29.81640625" customWidth="1"/>
+    <col min="6" max="7" width="33" customWidth="1"/>
+    <col min="8" max="8" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.81640625" customWidth="1"/>
+    <col min="10" max="10" width="38.26953125" customWidth="1"/>
+    <col min="11" max="11" width="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.81640625" customWidth="1"/>
+    <col min="14" max="14" width="76.81640625" customWidth="1"/>
+    <col min="15" max="15" width="34.26953125" customWidth="1"/>
+    <col min="16" max="16" width="43.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.1796875" customWidth="1"/>
+    <col min="22" max="22" width="36" customWidth="1"/>
+    <col min="23" max="23" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="52.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="40.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="48.90625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="31.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:37" ht="17" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AB1" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="AC1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="AE1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="AJ1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
-        <v>46</v>
-      </c>
       <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
         <v>2</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>7</v>
-      </c>
-      <c r="O2" t="s">
-        <v>8</v>
       </c>
       <c r="P2" t="s">
         <v>8</v>
       </c>
       <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
-        <v>47</v>
-      </c>
       <c r="T2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="U2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="V2" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="W2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="X2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="Y2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z2" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" t="s">
-        <v>39</v>
-      </c>
       <c r="AB2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC2" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" t="s">
-        <v>55</v>
-      </c>
       <c r="AE2" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="AF2" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="AG2" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="AH2" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="AI2" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="Y4">
+        <v>24</v>
+      </c>
+      <c r="AF4">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>